<commit_message>
sort function has been used
</commit_message>
<xml_diff>
--- a/unique.xlsx
+++ b/unique.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LEARN MS OFFICE\EXCEL\excel practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6073DB47-0158-4C06-A41A-61E14B884383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E0D6ED-7E37-4C64-B2D0-E9C86778E6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0290681B-6CD5-406B-BD22-BB674C3850CA}"/>
   </bookViews>
@@ -33,6 +33,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
@@ -55,8 +77,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -71,10 +101,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF404040"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Var(--ds-font-family-code)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -97,13 +127,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,15 +453,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DBF86B-8CA8-48D4-ACEE-6C6DA77C2613}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="8.7265625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,44 +473,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>1001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>1002</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>1003</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>1004</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>1005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="str" cm="1">
+        <f t="array" ref="A9:A11">_xlfn.UNIQUE(A2:A6)</f>
+        <v>John Doe</v>
+      </c>
+      <c r="B9" s="4" t="e" cm="1">
+        <f t="array" ref="B9">file</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="str">
+        <v>Jane Smith</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="str">
+        <v>Alice Johnson</v>
       </c>
     </row>
   </sheetData>

</xml_diff>